<commit_message>
añadidos ejercicios PHP y excel 06 de noviembre
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191105/datos practica6.xlsx
+++ b/m1/unidad3/Practicas/20191105/datos practica6.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.3374986342644544E-2"/>
+                  <c:y val="-4.1767814674970059E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1149,7 +1154,7 @@
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="none" lIns="540000" tIns="19050" rIns="36000" bIns="19050" anchor="ctr" anchorCtr="1">
                   <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
@@ -1170,7 +1175,7 @@
                   <a:endParaRPr lang="es-ES"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="l"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1181,7 +1186,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="3.3072877582502512E-2"/>
+                      <c:w val="9.4470546361900734E-2"/>
                       <c:h val="3.9663014892507162E-2"/>
                     </c:manualLayout>
                   </c15:layout>
@@ -1192,8 +1197,147 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="6"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="108000" tIns="19050" rIns="36000" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-F002-4E3D-8ADB-2F967333808A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="36000" bIns="36000" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F002-4E3D-8ADB-2F967333808A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="8"/>
               <c:layout/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="432000" tIns="19050" rIns="36000" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1203,6 +1347,15 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
                   <c15:layout/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1218,7 +1371,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="36000" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1249,22 +1402,17 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -2793,7 +2941,17 @@
       </c:spPr>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8368564565476931E-2"/>
+          <c:y val="7.7124173975067795E-2"/>
+          <c:w val="0.7615195294542827"/>
+          <c:h val="0.82903827511369954"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -2903,6 +3061,110 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.4575705581686312E-3"/>
+                  <c:y val="-4.1783442340412334E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-3FE9-443E-959E-046F7FEF217C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7753742383976401E-2"/>
+                  <c:y val="2.5070065404247249E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-3FE9-443E-959E-046F7FEF217C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.3194674872217085E-2"/>
+                  <c:y val="0.15668790877654626"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-3FE9-443E-959E-046F7FEF217C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0465889593132742E-2"/>
+                  <c:y val="-9.6101917382948376E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-3FE9-443E-959E-046F7FEF217C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -6404,7 +6666,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6448,7 +6710,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>